<commit_message>
modifications to excel file
</commit_message>
<xml_diff>
--- a/cea/databases/Technology-cost-database.xlsx
+++ b/cea/databases/Technology-cost-database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Technology Name</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>x is in Watts</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>Solar Collector</t>
@@ -483,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -542,7 +539,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>84000</v>
@@ -583,7 +580,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>35100</v>
@@ -618,7 +615,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <v>20300</v>
@@ -645,9 +642,41 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>32978</v>
+      </c>
+      <c r="E5">
+        <v>0.59670000000000001</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5">
+        <v>25</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
@@ -656,48 +685,83 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>32978</v>
+        <v>1209.5905171657048</v>
       </c>
       <c r="E6">
-        <v>0.59670000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="F6" s="1">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="G6" t="s">
         <v>28</v>
       </c>
       <c r="I6">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M6">
         <v>1</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>12000</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1209.5905171657048</v>
+        <v>3500</v>
       </c>
       <c r="E8">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1">
         <v>0.05</v>
       </c>
-      <c r="G8" t="s">
-        <v>28</v>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
       </c>
       <c r="I8">
         <v>20</v>
@@ -706,21 +770,50 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2500</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9">
+        <v>20</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>12000</v>
+        <v>2050</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -732,140 +825,44 @@
         <v>28</v>
       </c>
       <c r="I10">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="M10">
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
         <v>0</v>
       </c>
-      <c r="D12">
-        <v>3500</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12">
+      <c r="D11">
+        <v>5000</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11">
         <v>20</v>
       </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>2500</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13">
-        <v>20</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>2050</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15">
-        <v>20</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>5000</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17">
-        <v>20</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17" t="s">
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
seperate the database into conversion/storage/distribution technologies
</commit_message>
<xml_diff>
--- a/cea/databases/Technology-cost-database.xlsx
+++ b/cea/databases/Technology-cost-database.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Database" sheetId="1" r:id="rId1"/>
-    <sheet name="Reference" sheetId="2" r:id="rId2"/>
+    <sheet name="Conversion" sheetId="1" r:id="rId1"/>
+    <sheet name="Storage" sheetId="3" r:id="rId2"/>
+    <sheet name="Distribution" sheetId="4" r:id="rId3"/>
+    <sheet name="Reference" sheetId="2" r:id="rId4"/>
+    <sheet name="Equations" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
   <si>
     <t>Technology Name</t>
   </si>
@@ -103,9 +106,6 @@
     <t>City Energy Analyst: Integrated framework for analysis and optimization of building energy systems in neighborhoods and city districts</t>
   </si>
   <si>
-    <t>Combined Gas cycle turbine</t>
-  </si>
-  <si>
     <t>No range</t>
   </si>
   <si>
@@ -121,30 +121,12 @@
     <t>Photovoltaic Panels</t>
   </si>
   <si>
-    <t>10kW</t>
-  </si>
-  <si>
-    <t>200kW</t>
-  </si>
-  <si>
-    <t>x is in kW</t>
-  </si>
-  <si>
-    <t>x is in Watts</t>
-  </si>
-  <si>
-    <t>Solar Collector</t>
-  </si>
-  <si>
     <t>PV-thermal</t>
   </si>
   <si>
     <t>B1</t>
   </si>
   <si>
-    <t>CGCT1</t>
-  </si>
-  <si>
     <t>HEX1</t>
   </si>
   <si>
@@ -158,6 +140,66 @@
   </si>
   <si>
     <t>PVT1</t>
+  </si>
+  <si>
+    <t>capacity_min</t>
+  </si>
+  <si>
+    <t>capacity_max</t>
+  </si>
+  <si>
+    <t>Equation</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Equation number</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>O1</t>
+  </si>
+  <si>
+    <t>investment</t>
+  </si>
+  <si>
+    <t>operation</t>
+  </si>
+  <si>
+    <t>OC_Fixed*x + OC_variable*(utilities)</t>
+  </si>
+  <si>
+    <t>Combined Cycle Gas Turbine</t>
+  </si>
+  <si>
+    <t>CCGT1</t>
+  </si>
+  <si>
+    <t>Solar Thermal Collectors</t>
+  </si>
+  <si>
+    <t>x_unit</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>x_min</t>
+  </si>
+  <si>
+    <t>x_max</t>
   </si>
 </sst>
 </file>
@@ -193,13 +235,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,20 +528,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,13 +561,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
@@ -525,21 +576,24 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>84000</v>
@@ -550,23 +604,23 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="G2">
+      <c r="F2">
         <v>320000</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" t="s">
         <v>24</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="I2">
         <v>20</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>36</v>
+      <c r="K2" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
       </c>
       <c r="P2" t="s">
         <v>13</v>
@@ -578,9 +632,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>35100</v>
@@ -591,19 +645,19 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="1">
-        <v>0.05</v>
+      <c r="F3">
+        <v>90000</v>
       </c>
       <c r="G3">
-        <v>90000</v>
-      </c>
-      <c r="H3">
         <v>320000</v>
       </c>
       <c r="I3">
         <v>20</v>
       </c>
-      <c r="M3">
+      <c r="K3" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="N3">
         <v>1</v>
       </c>
       <c r="P3" t="s">
@@ -613,9 +667,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C4">
         <v>20300</v>
@@ -626,28 +680,28 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="1">
-        <v>0.05</v>
+      <c r="F4">
+        <v>28000</v>
       </c>
       <c r="G4">
-        <v>28000</v>
-      </c>
-      <c r="H4">
         <v>90000</v>
       </c>
       <c r="I4">
         <v>20</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="K4" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -658,212 +712,183 @@
       <c r="E5">
         <v>0.59670000000000001</v>
       </c>
-      <c r="F5" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>55</v>
       </c>
       <c r="I5">
         <v>25</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="K5" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1209.5905171657048</v>
+        <v>12000</v>
       </c>
       <c r="E6">
-        <v>0.6</v>
-      </c>
-      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="K6" s="1">
         <v>0.05</v>
       </c>
-      <c r="G6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6">
-        <v>20</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>12000</v>
+        <v>3500</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7">
+        <v>20</v>
+      </c>
+      <c r="K7" s="1">
         <v>0.05</v>
       </c>
-      <c r="G7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7">
-        <v>10</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>3500</v>
+        <v>2500</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="1">
-        <v>0.05</v>
+      <c r="F8">
+        <v>10</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I8">
         <v>20</v>
       </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="K8" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>2500</v>
+        <v>2050</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="G9" t="s">
-        <v>33</v>
+      <c r="F9" t="s">
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="I9">
         <v>20</v>
       </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="K9" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>2050</v>
+        <v>5000</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
       </c>
       <c r="I10">
         <v>20</v>
       </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>5000</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="K10" s="1">
         <v>0.05</v>
       </c>
-      <c r="G11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11">
-        <v>20</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11" t="s">
-        <v>35</v>
+      <c r="N10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -873,20 +898,176 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1209.5905171657048</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="4">
+        <v>20</v>
+      </c>
+      <c r="M2" s="4">
+        <v>1</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -903,7 +1084,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -915,6 +1096,65 @@
       </c>
       <c r="D2">
         <v>2016</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small updates in database structure
</commit_message>
<xml_diff>
--- a/cea/databases/Technology-cost-database.xlsx
+++ b/cea/databases/Technology-cost-database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Conversion" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="102">
   <si>
     <t>Technology Name</t>
   </si>
@@ -308,16 +308,28 @@
     <t xml:space="preserve">Labour cost </t>
   </si>
   <si>
-    <t xml:space="preserve">Fuel cost </t>
-  </si>
-  <si>
-    <t>Operation&amp; Maintanence cost</t>
-  </si>
-  <si>
     <t>capital cost/ usage</t>
   </si>
   <si>
     <t>Note on the variables</t>
+  </si>
+  <si>
+    <t>Financial cost</t>
+  </si>
+  <si>
+    <t>CAPEX</t>
+  </si>
+  <si>
+    <t>OPEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility cost </t>
+  </si>
+  <si>
+    <t>Interest rate</t>
+  </si>
+  <si>
+    <t>Pumps</t>
   </si>
 </sst>
 </file>
@@ -645,23 +657,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="3" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="2" max="3" width="12.26953125" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
-    <col min="16" max="17" width="14.42578125" customWidth="1"/>
+    <col min="16" max="18" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -714,10 +726,13 @@
         <v>54</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -748,20 +763,20 @@
       <c r="K2">
         <v>20</v>
       </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
         <v>11</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>12</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>30</v>
       </c>
@@ -786,17 +801,17 @@
       <c r="K3">
         <v>20</v>
       </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
         <v>13</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>30</v>
       </c>
@@ -821,11 +836,11 @@
       <c r="K4">
         <v>20</v>
       </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -850,11 +865,11 @@
       <c r="K5">
         <v>20</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -882,11 +897,11 @@
       <c r="K6">
         <v>25</v>
       </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -914,11 +929,11 @@
       <c r="K7">
         <v>10</v>
       </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -949,11 +964,11 @@
       <c r="K8">
         <v>20</v>
       </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>33</v>
       </c>
@@ -981,11 +996,11 @@
       <c r="K9">
         <v>20</v>
       </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1011,7 +1026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1039,11 +1054,11 @@
       <c r="K11">
         <v>20</v>
       </c>
-      <c r="R11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1071,7 +1086,7 @@
       <c r="K12">
         <v>20</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>1</v>
       </c>
     </row>
@@ -1088,18 +1103,18 @@
       <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="14" max="16" width="18.7109375" customWidth="1"/>
+    <col min="14" max="16" width="18.7265625" customWidth="1"/>
     <col min="17" max="17" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1152,7 +1167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1184,7 +1199,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1216,7 +1231,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
@@ -1227,20 +1242,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1293,7 +1308,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -1328,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1346,6 +1361,11 @@
       </c>
       <c r="J3" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1357,19 +1377,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="34.54296875" customWidth="1"/>
+    <col min="4" max="4" width="49.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -1380,10 +1400,10 @@
         <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1397,7 +1417,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1408,7 +1428,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1422,7 +1442,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -1449,14 +1469,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="79.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1473,7 +1493,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1487,7 +1507,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1501,7 +1521,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1522,20 +1542,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="53.28515625" customWidth="1"/>
+    <col min="2" max="2" width="53.26953125" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -1546,9 +1566,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>89</v>
@@ -1557,7 +1577,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>90</v>
       </c>
@@ -1565,31 +1585,36 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>95</v>
-      </c>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
         <v>93</v>
-      </c>
-      <c r="C4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>94</v>
       </c>
       <c r="C5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
         <v>79</v>
       </c>
-      <c r="C6" t="s">
-        <v>96</v>
+      <c r="C7" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>